<commit_message>
working model link layer builder
</commit_message>
<xml_diff>
--- a/layer-building/model_links/model_link_data_dict.xlsx
+++ b/layer-building/model_links/model_link_data_dict.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dconly\GitRepos\PPA3\layer-building\model_links\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92E03F65-3D12-478C-B9DF-744E07D89844}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF071ADA-4822-4B31-ABE7-3410469D3549}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="1" r:id="rId1"/>
@@ -13081,7 +13081,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="0.00000"/>
+    <numFmt numFmtId="164" formatCode="0.00000"/>
   </numFmts>
   <fonts count="12" x14ac:knownFonts="1">
     <font>
@@ -13223,7 +13223,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -13532,7 +13532,7 @@
   <dimension ref="A1:J132"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>